<commit_message>
Restoring the stashed changes
</commit_message>
<xml_diff>
--- a/Scripts/TC_ACC_08/Default.xlsx
+++ b/Scripts/TC_ACC_08/Default.xlsx
@@ -227,10 +227,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFFFF"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="283845"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>

</xml_diff>

<commit_message>
Sample test scripts are deleted
New scripts are developed
</commit_message>
<xml_diff>
--- a/Scripts/TC_ACC_08/Default.xlsx
+++ b/Scripts/TC_ACC_08/Default.xlsx
@@ -15,15 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
   <si>
-    <t>Qatar@2021</t>
+    <t>B</t>
   </si>
   <si>
-    <t>USERNAME</t>
-  </si>
-  <si>
-    <t>PASSWORD</t>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -168,7 +165,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -176,43 +173,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -511,16 +478,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="10.640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.49609375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.41796875" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -529,14 +495,6 @@
         <v>1</v>
       </c>
       <c t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row>
-      <c s="3">
-        <v>88996</v>
-      </c>
-      <c s="2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>